<commit_message>
Add Final ROA Code
</commit_message>
<xml_diff>
--- a/supervised-learning/charts/Weka-Parameters-Breast-Cancer.xlsx
+++ b/supervised-learning/charts/Weka-Parameters-Breast-Cancer.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohanrk/Desktop/College_Documents/Georgia Tech/Courses/Spring 2019/CS 4641/Assignment 1 - Supervised Learning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohanrk/Desktop/College_Documents/Georgia Tech/Courses/Spring 2019/CS 4641/Machine-Learning-4641/supervised-learning/charts/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="1560" windowWidth="24880" windowHeight="16720" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="3760" yWindow="500" windowWidth="24880" windowHeight="16720" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="J48 (Decision Tree)" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="34">
   <si>
     <t>Confidence Factor</t>
   </si>
@@ -411,11 +411,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1277989376"/>
-        <c:axId val="-1277985344"/>
+        <c:axId val="771135488"/>
+        <c:axId val="767199424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1277989376"/>
+        <c:axId val="771135488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -527,7 +527,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1277985344"/>
+        <c:crossAx val="767199424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -535,7 +535,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1277985344"/>
+        <c:axId val="767199424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -641,7 +641,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1277989376"/>
+        <c:crossAx val="771135488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -903,11 +903,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1277963856"/>
-        <c:axId val="-1277959824"/>
+        <c:axId val="770357648"/>
+        <c:axId val="767198272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1277963856"/>
+        <c:axId val="770357648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1024,7 +1024,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1277959824"/>
+        <c:crossAx val="767198272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1032,7 +1032,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1277959824"/>
+        <c:axId val="767198272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1138,7 +1138,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1277963856"/>
+        <c:crossAx val="770357648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1405,11 +1405,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1283089104"/>
-        <c:axId val="-1283042720"/>
+        <c:axId val="767093232"/>
+        <c:axId val="767096624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1283089104"/>
+        <c:axId val="767093232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1526,7 +1526,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1283042720"/>
+        <c:crossAx val="767096624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1534,7 +1534,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1283042720"/>
+        <c:axId val="767096624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1640,7 +1640,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1283089104"/>
+        <c:crossAx val="767093232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1768,6 +1768,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1910,11 +1911,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1282909152"/>
-        <c:axId val="-1282905120"/>
+        <c:axId val="766662896"/>
+        <c:axId val="766666288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1282909152"/>
+        <c:axId val="766662896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1965,6 +1966,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2031,7 +2033,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1282905120"/>
+        <c:crossAx val="766666288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2039,7 +2041,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1282905120"/>
+        <c:axId val="766666288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2085,6 +2087,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2145,7 +2148,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1282909152"/>
+        <c:crossAx val="766662896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2159,6 +2162,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2609,11 +2613,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1282865120"/>
-        <c:axId val="-1282861088"/>
+        <c:axId val="771978096"/>
+        <c:axId val="771982128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1282865120"/>
+        <c:axId val="771978096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2712,7 +2716,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1282861088"/>
+        <c:crossAx val="771982128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2720,7 +2724,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1282861088"/>
+        <c:axId val="771982128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2802,7 +2806,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1282865120"/>
+        <c:crossAx val="771978096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7079,7 +7083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -7646,10 +7650,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="87" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" zoomScalePageLayoutView="87" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8033,31 +8037,31 @@
         <v>0.1</v>
       </c>
       <c r="C14">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D14">
-        <v>600</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
         <v>17</v>
       </c>
       <c r="F14">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="G14" s="1">
-        <v>0.69346699999999994</v>
+        <v>0.73869300000000004</v>
       </c>
       <c r="H14">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="I14" s="1">
-        <v>0.306533</v>
+        <v>0.26130700000000001</v>
       </c>
       <c r="J14">
-        <v>0.31940000000000002</v>
+        <v>0.29959999999999998</v>
       </c>
       <c r="K14">
-        <v>0.5161</v>
+        <v>0.439</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -8065,31 +8069,31 @@
         <v>0.1</v>
       </c>
       <c r="C15">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D15">
-        <v>700</v>
+        <v>100</v>
       </c>
       <c r="E15" t="s">
         <v>17</v>
       </c>
       <c r="F15">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="G15" s="1">
-        <v>0.688442</v>
+        <v>0.73869300000000004</v>
       </c>
       <c r="H15">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="I15" s="1">
-        <v>0.311558</v>
+        <v>0.26130700000000001</v>
       </c>
       <c r="J15">
-        <v>0.31879999999999997</v>
+        <v>0.3029</v>
       </c>
       <c r="K15">
-        <v>0.51690000000000003</v>
+        <v>0.45800000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -8097,31 +8101,31 @@
         <v>0.1</v>
       </c>
       <c r="C16">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D16">
-        <v>800</v>
+        <v>200</v>
       </c>
       <c r="E16" t="s">
         <v>17</v>
       </c>
       <c r="F16">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G16" s="1">
-        <v>0.688442</v>
+        <v>0.698492</v>
       </c>
       <c r="H16">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I16" s="1">
-        <v>0.311558</v>
+        <v>0.301508</v>
       </c>
       <c r="J16">
-        <v>0.31840000000000002</v>
+        <v>0.31080000000000002</v>
       </c>
       <c r="K16">
-        <v>0.51759999999999995</v>
+        <v>0.49130000000000001</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
@@ -8129,31 +8133,31 @@
         <v>0.1</v>
       </c>
       <c r="C17">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D17">
-        <v>900</v>
+        <v>300</v>
       </c>
       <c r="E17" t="s">
         <v>17</v>
       </c>
       <c r="F17">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G17" s="1">
-        <v>0.688442</v>
+        <v>0.70351799999999998</v>
       </c>
       <c r="H17">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I17" s="1">
-        <v>0.311558</v>
+        <v>0.29648200000000002</v>
       </c>
       <c r="J17">
-        <v>0.31809999999999999</v>
+        <v>0.31109999999999999</v>
       </c>
       <c r="K17">
-        <v>0.5181</v>
+        <v>0.50229999999999997</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
@@ -8161,31 +8165,63 @@
         <v>0.1</v>
       </c>
       <c r="C18">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D18">
-        <v>1000</v>
+        <v>400</v>
       </c>
       <c r="E18" t="s">
         <v>17</v>
       </c>
       <c r="F18">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="G18" s="1">
-        <v>0.68341700000000005</v>
+        <v>0.70351799999999998</v>
       </c>
       <c r="H18">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I18" s="1">
-        <v>0.316583</v>
+        <v>0.29648200000000002</v>
       </c>
       <c r="J18">
-        <v>0.31780000000000003</v>
+        <v>0.31269999999999998</v>
       </c>
       <c r="K18">
-        <v>0.51859999999999995</v>
+        <v>0.50549999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>0.1</v>
+      </c>
+      <c r="C19">
+        <v>0.2</v>
+      </c>
+      <c r="D19">
+        <v>500</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19">
+        <v>139</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.698492</v>
+      </c>
+      <c r="H19">
+        <v>60</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.301508</v>
+      </c>
+      <c r="J19">
+        <v>0.3201</v>
+      </c>
+      <c r="K19">
+        <v>0.51480000000000004</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
@@ -8193,31 +8229,31 @@
         <v>0.1</v>
       </c>
       <c r="C20">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D20">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="E20" t="s">
         <v>17</v>
       </c>
       <c r="F20">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G20" s="1">
-        <v>0.698492</v>
+        <v>0.69346699999999994</v>
       </c>
       <c r="H20">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I20" s="1">
-        <v>0.301508</v>
+        <v>0.306533</v>
       </c>
       <c r="J20">
-        <v>0.31269999999999998</v>
+        <v>0.31940000000000002</v>
       </c>
       <c r="K20">
-        <v>0.50660000000000005</v>
+        <v>0.5161</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
@@ -8225,31 +8261,31 @@
         <v>0.1</v>
       </c>
       <c r="C21">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D21">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="E21" t="s">
         <v>17</v>
       </c>
       <c r="F21">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G21" s="1">
-        <v>0.71356799999999998</v>
+        <v>0.688442</v>
       </c>
       <c r="H21">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="I21" s="1">
-        <v>0.28643200000000002</v>
+        <v>0.311558</v>
       </c>
       <c r="J21">
-        <v>0.31069999999999998</v>
+        <v>0.31879999999999997</v>
       </c>
       <c r="K21">
-        <v>0.50560000000000005</v>
+        <v>0.51690000000000003</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
@@ -8257,31 +8293,31 @@
         <v>0.1</v>
       </c>
       <c r="C22">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="D22">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="E22" t="s">
         <v>17</v>
       </c>
       <c r="F22">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G22" s="1">
-        <v>0.70351799999999998</v>
+        <v>0.688442</v>
       </c>
       <c r="H22">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I22" s="1">
-        <v>0.29648200000000002</v>
+        <v>0.311558</v>
       </c>
       <c r="J22">
-        <v>0.32150000000000001</v>
+        <v>0.31840000000000002</v>
       </c>
       <c r="K22">
-        <v>0.51349999999999996</v>
+        <v>0.51759999999999995</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
@@ -8289,31 +8325,31 @@
         <v>0.1</v>
       </c>
       <c r="C23">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="D23">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="E23" t="s">
         <v>17</v>
       </c>
       <c r="F23">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="G23" s="1">
-        <v>0.67336700000000005</v>
+        <v>0.688442</v>
       </c>
       <c r="H23">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I23" s="1">
-        <v>0.32663300000000001</v>
+        <v>0.311558</v>
       </c>
       <c r="J23">
-        <v>0.33310000000000001</v>
+        <v>0.31809999999999999</v>
       </c>
       <c r="K23">
-        <v>0.52900000000000003</v>
+        <v>0.5181</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
@@ -8321,63 +8357,31 @@
         <v>0.1</v>
       </c>
       <c r="C24">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="D24">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E24" t="s">
         <v>17</v>
       </c>
       <c r="F24">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="G24" s="1">
-        <v>0.65326600000000001</v>
+        <v>0.68341700000000005</v>
       </c>
       <c r="H24">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="I24" s="1">
-        <v>0.34673399999999999</v>
+        <v>0.316583</v>
       </c>
       <c r="J24">
-        <v>0.34720000000000001</v>
+        <v>0.31780000000000003</v>
       </c>
       <c r="K24">
-        <v>0.53800000000000003</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25">
-        <v>0.1</v>
-      </c>
-      <c r="C25">
-        <v>0.8</v>
-      </c>
-      <c r="D25">
-        <v>500</v>
-      </c>
-      <c r="E25" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25">
-        <v>137</v>
-      </c>
-      <c r="G25" s="1">
-        <v>0.688442</v>
-      </c>
-      <c r="H25">
-        <v>62</v>
-      </c>
-      <c r="I25" s="1">
-        <v>0.311558</v>
-      </c>
-      <c r="J25">
-        <v>0.3165</v>
-      </c>
-      <c r="K25">
-        <v>0.52159999999999995</v>
+        <v>0.51859999999999995</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
@@ -8385,7 +8389,7 @@
         <v>0.1</v>
       </c>
       <c r="C26">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="D26">
         <v>500</v>
@@ -8394,22 +8398,22 @@
         <v>17</v>
       </c>
       <c r="F26">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="G26" s="1">
-        <v>0.65326600000000001</v>
+        <v>0.698492</v>
       </c>
       <c r="H26">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="I26" s="1">
-        <v>0.34673399999999999</v>
+        <v>0.301508</v>
       </c>
       <c r="J26">
-        <v>0.34939999999999999</v>
+        <v>0.31269999999999998</v>
       </c>
       <c r="K26">
-        <v>0.55700000000000005</v>
+        <v>0.50660000000000005</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
@@ -8417,7 +8421,7 @@
         <v>0.1</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D27">
         <v>500</v>
@@ -8426,22 +8430,54 @@
         <v>17</v>
       </c>
       <c r="F27">
+        <v>142</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.71356799999999998</v>
+      </c>
+      <c r="H27">
+        <v>57</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0.28643200000000002</v>
+      </c>
+      <c r="J27">
+        <v>0.31069999999999998</v>
+      </c>
+      <c r="K27">
+        <v>0.50560000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>0.1</v>
+      </c>
+      <c r="C28">
+        <v>0.5</v>
+      </c>
+      <c r="D28">
+        <v>500</v>
+      </c>
+      <c r="E28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28">
         <v>140</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G28" s="1">
         <v>0.70351799999999998</v>
       </c>
-      <c r="H27">
+      <c r="H28">
         <v>59</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I28" s="1">
         <v>0.29648200000000002</v>
       </c>
-      <c r="J27">
-        <v>0.29649999999999999</v>
-      </c>
-      <c r="K27">
-        <v>0.54449999999999998</v>
+      <c r="J28">
+        <v>0.32150000000000001</v>
+      </c>
+      <c r="K28">
+        <v>0.51349999999999996</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
@@ -8449,31 +8485,31 @@
         <v>0.1</v>
       </c>
       <c r="C29">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D29">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="E29" t="s">
         <v>17</v>
       </c>
       <c r="F29">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G29" s="1">
-        <v>0.70351799999999998</v>
+        <v>0.67336700000000005</v>
       </c>
       <c r="H29">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="I29" s="1">
-        <v>0.29648200000000002</v>
+        <v>0.32663300000000001</v>
       </c>
       <c r="J29">
-        <v>0.31269999999999998</v>
+        <v>0.33310000000000001</v>
       </c>
       <c r="K29">
-        <v>0.50549999999999995</v>
+        <v>0.52900000000000003</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
@@ -8481,31 +8517,31 @@
         <v>0.1</v>
       </c>
       <c r="C30">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="D30">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E30" t="s">
         <v>17</v>
       </c>
       <c r="F30">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="G30" s="1">
-        <v>0.70351799999999998</v>
+        <v>0.65326600000000001</v>
       </c>
       <c r="H30">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="I30" s="1">
-        <v>0.29648200000000002</v>
+        <v>0.34673399999999999</v>
       </c>
       <c r="J30">
-        <v>0.31109999999999999</v>
+        <v>0.34720000000000001</v>
       </c>
       <c r="K30">
-        <v>0.50229999999999997</v>
+        <v>0.53800000000000003</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
@@ -8513,31 +8549,31 @@
         <v>0.1</v>
       </c>
       <c r="C31">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D31">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="E31" t="s">
         <v>17</v>
       </c>
       <c r="F31">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G31" s="1">
-        <v>0.698492</v>
+        <v>0.688442</v>
       </c>
       <c r="H31">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I31" s="1">
-        <v>0.301508</v>
+        <v>0.311558</v>
       </c>
       <c r="J31">
-        <v>0.31080000000000002</v>
+        <v>0.3165</v>
       </c>
       <c r="K31">
-        <v>0.49130000000000001</v>
+        <v>0.52159999999999995</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
@@ -8545,31 +8581,31 @@
         <v>0.1</v>
       </c>
       <c r="C32">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D32">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="E32" t="s">
         <v>17</v>
       </c>
       <c r="F32">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="G32" s="1">
-        <v>0.73869300000000004</v>
+        <v>0.65326600000000001</v>
       </c>
       <c r="H32">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="I32" s="1">
-        <v>0.26130700000000001</v>
+        <v>0.34673399999999999</v>
       </c>
       <c r="J32">
-        <v>0.3029</v>
+        <v>0.34939999999999999</v>
       </c>
       <c r="K32">
-        <v>0.45800000000000002</v>
+        <v>0.55700000000000005</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -8577,79 +8613,102 @@
         <v>0.1</v>
       </c>
       <c r="C33">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="D33">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="E33" t="s">
         <v>17</v>
       </c>
       <c r="F33">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G33" s="1">
-        <v>0.73869300000000004</v>
+        <v>0.70351799999999998</v>
       </c>
       <c r="H33">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="I33" s="1">
-        <v>0.26130700000000001</v>
+        <v>0.29648200000000002</v>
       </c>
       <c r="J33">
-        <v>0.29959999999999998</v>
+        <v>0.29649999999999999</v>
       </c>
       <c r="K33">
-        <v>0.439</v>
+        <v>0.54449999999999998</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="G35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
         <v>12</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C42" t="s">
         <v>18</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D42" t="s">
         <v>13</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E42" t="s">
         <v>16</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F42" t="s">
         <v>14</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G42" t="s">
         <v>15</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H42" t="s">
         <v>5</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I42" t="s">
         <v>8</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J42" t="s">
         <v>6</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K42" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B37">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B43">
         <v>0.1</v>
       </c>
-      <c r="C37">
+      <c r="C43">
         <v>0.2</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="B29:K33">
+    <sortCondition ref="D29:D33"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9501,7 +9560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>

</xml_diff>